<commit_message>
Data got auto-formatted wrong by LibreOffice... fixed.
</commit_message>
<xml_diff>
--- a/data/awards.xlsx
+++ b/data/awards.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>award_name</t>
   </si>
@@ -169,9 +169,6 @@
     <t>2018 CL Davis Foundation Student Scholarship Award</t>
   </si>
   <si>
-    <t>05-11-2018</t>
-  </si>
-  <si>
     <t>Description to follow.</t>
   </si>
 </sst>
@@ -181,7 +178,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
@@ -303,7 +300,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="B2:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -696,14 +693,14 @@
       <c r="E18" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="n">
+        <v>43409</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>